<commit_message>
vitesse fiable OK !
</commit_message>
<xml_diff>
--- a/packageGES/data/impactCarbone.xlsx
+++ b/packageGES/data/impactCarbone.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hazelya\PycharmProjects\packageGES\packageGES\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1AA4B0-45D6-4A38-89C1-6F3F178D40B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FE2BE3-0267-40F2-B5F7-A138BB6F776B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -436,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -473,7 +473,7 @@
         <v>23</v>
       </c>
       <c r="D2" s="1">
-        <v>600</v>
+        <v>500</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -487,7 +487,7 @@
         <v>0.13</v>
       </c>
       <c r="D3" s="1">
-        <v>80</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -501,7 +501,7 @@
         <v>23</v>
       </c>
       <c r="D4" s="1">
-        <v>800</v>
+        <v>850</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -515,7 +515,7 @@
         <v>23</v>
       </c>
       <c r="D5" s="1">
-        <v>900</v>
+        <v>750</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -529,7 +529,7 @@
         <v>0.4</v>
       </c>
       <c r="D6" s="1">
-        <v>100</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -543,7 +543,7 @@
         <v>0.2</v>
       </c>
       <c r="D7" s="1">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
@@ -557,7 +557,7 @@
         <v>0.15</v>
       </c>
       <c r="D8" s="1">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -571,7 +571,7 @@
         <v>0.27</v>
       </c>
       <c r="D9" s="1">
-        <v>100</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -585,7 +585,7 @@
         <v>0.1</v>
       </c>
       <c r="D10" s="1">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
@@ -613,7 +613,7 @@
         <v>0</v>
       </c>
       <c r="D12" s="1">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
@@ -627,7 +627,7 @@
         <v>0</v>
       </c>
       <c r="D13" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -641,7 +641,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="1">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -655,7 +655,7 @@
         <v>0.1</v>
       </c>
       <c r="D15" s="1">
-        <v>100</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -669,7 +669,7 @@
         <v>0.01</v>
       </c>
       <c r="D16" s="1">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -683,7 +683,7 @@
         <v>0.24</v>
       </c>
       <c r="D17" s="1">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
@@ -697,7 +697,7 @@
         <v>0.104</v>
       </c>
       <c r="D18" s="1">
-        <v>300</v>
+        <v>158</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -711,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
@@ -725,7 +725,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="1">
-        <v>5</v>
+        <v>3.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mise a or prix
</commit_message>
<xml_diff>
--- a/packageGES/data/impactCarbone.xlsx
+++ b/packageGES/data/impactCarbone.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hazelya\PycharmProjects\packageGES\packageGES\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{029D38A3-5249-4B47-A0FE-3B2D0342BD65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00ABD4D-C2C5-4687-B956-1FEB48A09D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Voiture thermique</t>
   </si>
@@ -75,12 +75,6 @@
   </si>
   <si>
     <t>mode_transport</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Avion court courrier</t>
   </si>
   <si>
     <t>Moto thermique</t>
@@ -458,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,13 +471,13 @@
         <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>10</v>
@@ -494,168 +488,156 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" s="1">
-        <v>0.25819999999999999</v>
+        <v>0.1648</v>
       </c>
       <c r="C2" s="1">
-        <v>0.25857999999999998</v>
+        <v>0.1913</v>
       </c>
       <c r="D2" s="1">
-        <f>C2-B2</f>
-        <v>3.7999999999999146E-4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
+        <v>2.6499999999999999E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.13</v>
       </c>
       <c r="F2">
-        <v>600</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>0.1648</v>
+        <v>0.192</v>
       </c>
       <c r="C3" s="1">
-        <v>0.1913</v>
+        <v>0.21759999999999999</v>
       </c>
       <c r="D3" s="1">
-        <f>C3-B3</f>
-        <v>2.6499999999999996E-2</v>
+        <v>2.5600000000000001E-2</v>
       </c>
       <c r="E3">
-        <v>0.13</v>
+        <v>0.4</v>
       </c>
       <c r="F3" s="1">
-        <v>80</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1">
-        <v>0.192</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="C4" s="1">
-        <v>0.21759999999999999</v>
+        <v>0.10879999999999999</v>
       </c>
       <c r="D4" s="1">
-        <f>C4-B4</f>
-        <v>2.5599999999999984E-2</v>
+        <v>1.2800000000000001E-2</v>
       </c>
       <c r="E4">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="F4" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>7.2529999999999997E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8.5299999999999994E-3</v>
+      </c>
+      <c r="E5">
+        <v>0.133333333</v>
+      </c>
+      <c r="F5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="1">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0.10879999999999999</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" ref="D5:D27" si="0">C5-B5</f>
-        <v>1.2799999999999992E-2</v>
-      </c>
-      <c r="E5">
-        <f>0.4/2</f>
+      <c r="B6" s="1">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5.4399999999999997E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="E6">
+        <v>0.1</v>
+      </c>
+      <c r="F6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1">
+        <v>3.8399999999999997E-2</v>
+      </c>
+      <c r="C7" s="1">
+        <v>4.3520000000000003E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5.1200000000000004E-3</v>
+      </c>
+      <c r="E7">
+        <v>0.08</v>
+      </c>
+      <c r="F7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0.1043</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0.1132</v>
+      </c>
+      <c r="D8" s="1">
+        <v>8.8999999999999999E-3</v>
+      </c>
+      <c r="E8">
         <v>0.2</v>
       </c>
-      <c r="F5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="1">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>7.2529999999999997E-2</v>
-      </c>
-      <c r="D6" s="1">
-        <f t="shared" si="0"/>
-        <v>8.5299999999999959E-3</v>
-      </c>
-      <c r="E6">
-        <f>0.4/3</f>
-        <v>0.13333333333333333</v>
-      </c>
-      <c r="F6">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="1">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>5.4399999999999997E-2</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
-        <v>6.399999999999996E-3</v>
-      </c>
-      <c r="E7">
-        <f>0.4/4</f>
-        <v>0.1</v>
-      </c>
-      <c r="F7">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="1">
-        <v>3.8399999999999997E-2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>4.3520000000000003E-2</v>
-      </c>
-      <c r="D8" s="1">
-        <f t="shared" si="0"/>
-        <v>5.1200000000000065E-3</v>
-      </c>
-      <c r="E8">
-        <f>0.4/5</f>
-        <v>0.08</v>
-      </c>
       <c r="F8">
-        <v>100</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
-        <v>0.1043</v>
+        <v>0.1128</v>
       </c>
       <c r="C9" s="1">
-        <v>0.1132</v>
+        <v>0.1217</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="0"/>
-        <v>8.8999999999999913E-3</v>
+        <v>8.8999999999999999E-3</v>
       </c>
       <c r="E9">
         <v>0.2</v>
@@ -666,371 +648,341 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
-        <v>0.1128</v>
+        <v>6.0400000000000002E-2</v>
       </c>
       <c r="C10" s="1">
-        <v>0.1217</v>
+        <v>7.6300000000000007E-2</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="0"/>
-        <v>8.9000000000000051E-3</v>
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="E10">
+        <v>0.15</v>
       </c>
       <c r="F10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="B11" s="1">
-        <v>6.0400000000000002E-2</v>
+        <v>1.9800000000000002E-2</v>
       </c>
       <c r="C11" s="1">
-        <v>7.6300000000000007E-2</v>
+        <v>0.10340000000000001</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="0"/>
-        <v>1.5900000000000004E-2</v>
+        <v>8.3599999999999994E-2</v>
       </c>
       <c r="E11">
-        <v>0.15</v>
+        <v>0.27</v>
       </c>
       <c r="F11" s="1">
-        <v>45</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1">
-        <v>1.9800000000000002E-2</v>
+        <v>9.9000000000000008E-3</v>
       </c>
       <c r="C12" s="1">
-        <v>0.10340000000000001</v>
+        <v>5.1700000000000003E-2</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="0"/>
-        <v>8.3600000000000008E-2</v>
+        <v>4.1799999999999997E-2</v>
       </c>
       <c r="E12">
-        <v>0.27</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="F12" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="1">
+        <v>6.6E-3</v>
+      </c>
+      <c r="C13" s="1">
+        <v>3.4470000000000001E-2</v>
+      </c>
+      <c r="D13" s="1">
+        <v>2.7869999999999999E-2</v>
+      </c>
+      <c r="E13">
+        <v>0.09</v>
+      </c>
+      <c r="F13" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="1">
-        <v>9.9000000000000008E-3</v>
-      </c>
-      <c r="C13" s="1">
-        <v>5.1700000000000003E-2</v>
-      </c>
-      <c r="D13" s="1">
-        <f t="shared" si="0"/>
-        <v>4.1800000000000004E-2</v>
-      </c>
-      <c r="E13">
-        <f>0.27/2</f>
-        <v>0.13500000000000001</v>
-      </c>
-      <c r="F13" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1">
+        <v>4.9500000000000004E-3</v>
+      </c>
+      <c r="C14" s="1">
+        <v>2.5850000000000001E-2</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2.0899999999999998E-2</v>
+      </c>
+      <c r="E14">
+        <v>6.7500000000000004E-2</v>
+      </c>
+      <c r="F14" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="1">
-        <v>6.6E-3</v>
-      </c>
-      <c r="C14" s="1">
-        <v>3.4470000000000001E-2</v>
-      </c>
-      <c r="D14" s="1">
-        <f t="shared" si="0"/>
-        <v>2.7869999999999999E-2</v>
-      </c>
-      <c r="E14">
-        <f>0.27/3</f>
-        <v>9.0000000000000011E-2</v>
-      </c>
-      <c r="F14" s="1">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="B15" s="1">
-        <v>4.9500000000000004E-3</v>
+        <v>3.96E-3</v>
       </c>
       <c r="C15" s="1">
-        <v>2.5850000000000001E-2</v>
+        <v>2.068E-2</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
-        <v>2.0900000000000002E-2</v>
+        <v>1.6719999999999999E-2</v>
       </c>
       <c r="E15">
-        <f>0.27/4</f>
-        <v>6.7500000000000004E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="F15" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B16" s="1">
-        <v>3.96E-3</v>
+        <v>2.29E-2</v>
       </c>
       <c r="C16" s="1">
-        <v>2.068E-2</v>
+        <v>2.7689999999999999E-2</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="0"/>
-        <v>1.6719999999999999E-2</v>
+        <v>4.79E-3</v>
       </c>
       <c r="E16">
-        <f>0.27/5</f>
-        <v>5.4000000000000006E-2</v>
+        <v>0.1</v>
       </c>
       <c r="F16" s="1">
-        <v>100</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="B17" s="1">
-        <v>2.29E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="C17" s="1">
-        <v>2.7689999999999999E-2</v>
+        <v>2.9420000000000002E-2</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="0"/>
-        <v>4.7899999999999991E-3</v>
+        <v>4.4200000000000003E-3</v>
       </c>
       <c r="E17">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="F17" s="1">
-        <v>90</v>
+        <v>80</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1">
-        <v>2.5000000000000001E-2</v>
+        <v>2.2300000000000002E-3</v>
       </c>
       <c r="C18" s="1">
-        <v>2.9420000000000002E-2</v>
+        <v>1.095E-2</v>
       </c>
       <c r="D18" s="1">
-        <f>C18-B18</f>
-        <v>4.4200000000000003E-3</v>
+        <v>8.7200000000000003E-3</v>
+      </c>
+      <c r="E18">
+        <v>0.03</v>
       </c>
       <c r="F18" s="1">
-        <v>80</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="B19" s="1">
-        <v>2.2300000000000002E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="C19" s="1">
-        <v>1.095E-2</v>
+        <v>2.4899999999999999E-2</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="0"/>
-        <v>8.7199999999999986E-3</v>
+        <v>2.29E-2</v>
+      </c>
+      <c r="E19">
+        <v>0.02</v>
       </c>
       <c r="F19" s="1">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="B20" s="1">
-        <v>2E-3</v>
+        <v>6.6E-3</v>
       </c>
       <c r="C20" s="1">
-        <v>2.4899999999999999E-2</v>
+        <v>9.7800000000000005E-3</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="0"/>
-        <v>2.2899999999999997E-2</v>
+        <v>3.1800000000000001E-3</v>
+      </c>
+      <c r="E20">
+        <v>0.1</v>
       </c>
       <c r="F20" s="1">
-        <v>20</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="B21" s="1">
-        <v>6.6E-3</v>
+        <v>5.7999999999999996E-3</v>
       </c>
       <c r="C21" s="1">
-        <v>9.7800000000000005E-3</v>
+        <v>8.9800000000000001E-3</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="0"/>
-        <v>3.1800000000000005E-3</v>
-      </c>
-      <c r="E21" t="s">
-        <v>13</v>
+        <v>3.1800000000000001E-3</v>
+      </c>
+      <c r="E21">
+        <v>0.1</v>
       </c>
       <c r="F21" s="1">
-        <v>50</v>
+        <v>100</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1">
-        <v>5.7999999999999996E-3</v>
+        <v>4.1999999999999997E-3</v>
       </c>
       <c r="C22" s="1">
-        <v>8.9800000000000001E-3</v>
+        <v>4.4400000000000004E-3</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="0"/>
-        <v>3.1800000000000005E-3</v>
+        <v>2.4000000000000001E-4</v>
       </c>
       <c r="E22">
-        <v>0.1</v>
+        <v>0.01</v>
       </c>
       <c r="F22" s="1">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B23" s="1">
-        <v>4.1999999999999997E-3</v>
+        <v>3.8E-3</v>
       </c>
       <c r="C23" s="1">
-        <v>4.4400000000000004E-3</v>
+        <v>4.28E-3</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="0"/>
-        <v>2.4000000000000063E-4</v>
+        <v>4.8000000000000001E-4</v>
       </c>
       <c r="E23">
-        <v>0.01</v>
+        <v>0.24</v>
       </c>
       <c r="F23" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24" s="1">
-        <v>3.8E-3</v>
+        <v>2.3E-3</v>
       </c>
       <c r="C24" s="1">
-        <v>4.28E-3</v>
+        <v>2.9299999999999999E-3</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="0"/>
-        <v>4.7999999999999996E-4</v>
+        <v>6.3000000000000003E-4</v>
       </c>
       <c r="E24">
-        <v>0.24</v>
+        <v>0.104</v>
       </c>
       <c r="F24" s="1">
-        <v>20</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1">
-        <v>2.3E-3</v>
+        <v>0</v>
       </c>
       <c r="C25" s="1">
-        <v>2.9299999999999999E-3</v>
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="D25" s="1">
-        <f>C25-B25</f>
-        <v>6.2999999999999992E-4</v>
+        <v>1.7000000000000001E-4</v>
       </c>
       <c r="E25">
-        <v>0.104</v>
+        <v>0</v>
       </c>
       <c r="F25" s="1">
-        <v>300</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
       </c>
       <c r="C26" s="1">
-        <v>1.7000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="0"/>
-        <v>1.7000000000000001E-4</v>
+        <v>0</v>
       </c>
       <c r="E26">
         <v>0</v>
       </c>
       <c r="F26" s="1">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B27" s="1">
-        <v>0</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0</v>
-      </c>
-      <c r="D27" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <v>0</v>
-      </c>
-      <c r="F27" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>